<commit_message>
LAst Day in Lombok
</commit_message>
<xml_diff>
--- a/storage/app/public/template_upload/Format_Upload_Penduduk.xlsx
+++ b/storage/app/public/template_upload/Format_Upload_Penduduk.xlsx
@@ -13,14 +13,14 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PENDUDUK!$A$1:$S$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PENDUDUK!$A$1:$N$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>nik</t>
   </si>
@@ -64,21 +64,6 @@
     <t>alamat_sekarang</t>
   </si>
   <si>
-    <t>desa_id</t>
-  </si>
-  <si>
-    <t>kecamatan_id</t>
-  </si>
-  <si>
-    <t>kabupaten_id</t>
-  </si>
-  <si>
-    <t>provinsi_id</t>
-  </si>
-  <si>
-    <t>status_dasar</t>
-  </si>
-  <si>
     <t>1105073112520015</t>
   </si>
   <si>
@@ -95,13 +80,16 @@
   </si>
   <si>
     <t>1965-07-02</t>
+  </si>
+  <si>
+    <t>no_kk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,12 +97,6 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,9 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -502,14 +483,9 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,24 +529,12 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" t="s">
-        <v>19</v>
       </c>
       <c r="B2" t="str">
         <f>UPPER([1]Sheet1!B2)</f>
@@ -585,7 +549,7 @@
         <v>COT SUKON</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <f>IF([1]Sheet1!F2="A",1,IF([1]Sheet1!F2="B",2,IF([1]Sheet1!F2="AB",3,IF([1]Sheet1!F2="O",4,IF([1]Sheet1!F2="A+",5,IF([1]Sheet1!F2="A-",6,IF([1]Sheet1!F2="B+",7,IF([1]Sheet1!F2="B-",8,IF([1]Sheet1!F2="AB+",9,IF([1]Sheet1!F2="AB-",10,IF([1]Sheet1!F2="O+",11,IF([1]Sheet1!F2="O-",12,13))))))))))))</f>
@@ -607,33 +571,18 @@
         <v>81</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2">
-        <v>1107062011</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1107062</v>
-      </c>
-      <c r="Q2">
-        <v>1107</v>
-      </c>
-      <c r="R2">
-        <v>11</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B3" t="str">
         <f>UPPER([1]Sheet1!B3)</f>
@@ -648,7 +597,7 @@
         <v>TANGKEH</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <f>IF([1]Sheet1!F3="A",1,IF([1]Sheet1!F3="B",2,IF([1]Sheet1!F3="AB",3,IF([1]Sheet1!F3="O",4,IF([1]Sheet1!F3="A+",5,IF([1]Sheet1!F3="A-",6,IF([1]Sheet1!F3="B+",7,IF([1]Sheet1!F3="B-",8,IF([1]Sheet1!F3="AB+",9,IF([1]Sheet1!F3="AB-",10,IF([1]Sheet1!F3="O+",11,IF([1]Sheet1!F3="O-",12,13))))))))))))</f>
@@ -670,36 +619,22 @@
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3">
-        <v>1107062011</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1107062</v>
-      </c>
-      <c r="Q3">
-        <v>1107</v>
-      </c>
-      <c r="R3">
-        <v>11</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S3">
+  <autoFilter ref="A1:N3">
     <filterColumn colId="7"/>
     <filterColumn colId="9"/>
     <filterColumn colId="10"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>